<commit_message>
Add, put same titles to all, plus merge and main title headers add is complete
</commit_message>
<xml_diff>
--- a/Inventory_comparator/inventory_files/Contpaq.xlsx
+++ b/Inventory_comparator/inventory_files/Contpaq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualUnity\Documents\Inventory_comparator\inventory_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualUnity\Documents\GitHub\excel_tools\Inventory_comparator\inventory_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,19 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Part number</t>
-  </si>
-  <si>
-    <t>Quantities</t>
-  </si>
-  <si>
-    <t>Units of measurement</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>132d5f</t>
   </si>
@@ -72,6 +60,27 @@
   </si>
   <si>
     <t>mts</t>
+  </si>
+  <si>
+    <t>65dsf</t>
+  </si>
+  <si>
+    <t>345df</t>
+  </si>
+  <si>
+    <t>345dg</t>
+  </si>
+  <si>
+    <t>part number</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>UM</t>
+  </si>
+  <si>
+    <t>value mxn</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -119,6 +128,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +413,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,27 +424,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>2.54</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4">
         <v>0.15</v>
@@ -442,13 +452,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4">
         <v>0.2</v>
@@ -456,13 +466,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>100</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4">
         <v>0.32</v>
@@ -470,13 +480,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>61</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4">
         <v>0.8</v>
@@ -484,13 +494,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>500</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4">
         <v>0.42</v>
@@ -498,27 +508,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>1200</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4">
         <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>100000</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4">
         <v>0.98</v>
@@ -526,13 +536,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4">
         <v>1.2</v>
@@ -540,41 +550,73 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>680</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <v>800</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>80</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>